<commit_message>
Added invalid case role for organisation policy
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_invalid.xlsx
+++ b/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/BEFTA_Master_Definition_invalid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olawaleolanrewaju/Documents/Git_MOJ/befta-fw/src/main/resources/uk/gov/hmcts/befta/dse/ccd/definitions/invalid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC05532-9D7A-0745-B647-FE9AB75DB4A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3506C73D-DF6B-D949-BB07-30DFAF57027C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5618" uniqueCount="945">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5619" uniqueCount="946">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -2971,6 +2971,9 @@
   </si>
   <si>
     <t>Update a case</t>
+  </si>
+  <si>
+    <t>[INVALID]</t>
   </si>
 </sst>
 </file>
@@ -45255,7 +45258,9 @@
       <c r="F35" s="417" t="s">
         <v>915</v>
       </c>
-      <c r="G35" s="417"/>
+      <c r="G35" s="417" t="s">
+        <v>945</v>
+      </c>
       <c r="H35" s="417"/>
       <c r="I35" s="414"/>
       <c r="J35" s="414">

</xml_diff>